<commit_message>
modified:   backend/app.py 	modified:   backend/paperlbos.txt 	modified:   backend/prompt.txt 	modified:   backend/tester.py 	modified:   chatbot-app/node_modules/.cache/.eslintcache 	new file:   chatbot-app/node_modules/.cache/babel-loader/2d1de8395c4b4d87cc46d729581a260b9b7a65c133a4cdf07ecae400e322e7a0.json 	modified:   chatbot-app/node_modules/.cache/default-development/0.pack 	modified:   chatbot-app/node_modules/.cache/default-development/1.pack 	modified:   chatbot-app/node_modules/.cache/default-development/index.pack 	modified:   chatbot-app/node_modules/.cache/default-development/index.pack.old 	modified:   output.xlsx
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,41 +422,20 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>entry_multiple</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 6</t>
-        </is>
-      </c>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr"/>
+      <c r="F1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -485,7 +452,6 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -502,7 +468,6 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -519,7 +484,6 @@
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -536,7 +500,6 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -546,14 +509,13 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -570,7 +532,6 @@
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -587,71 +548,70 @@
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EBITDA Y1</t>
-        </is>
-      </c>
-      <c r="B9">
-        <f>$B$3*$B$2</f>
-        <v/>
+          <t>tax_rate</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>price_paid</t>
-        </is>
-      </c>
-      <c r="B10">
-        <f>$B$1*$B$15</f>
-        <v/>
+          <t>capex_per_of_rev</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>debt_portion</t>
-        </is>
-      </c>
-      <c r="B11">
-        <f>$B$4*$B$16</f>
-        <v/>
+          <t>change_in_NWC</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>5000000</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>equity_portion</t>
-        </is>
-      </c>
-      <c r="B12">
-        <f>$B$5*$B$16</f>
-        <v/>
+          <t>depreciation</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>20000000</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -660,7 +620,6 @@
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -669,480 +628,423 @@
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
+          <t>EBITDA Y1</t>
+        </is>
+      </c>
+      <c r="B15">
+        <f>$B$3*$B$2</f>
+        <v/>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Rev</t>
+          <t>price_paid</t>
         </is>
       </c>
       <c r="B16">
-        <f>$B$2</f>
-        <v/>
-      </c>
-      <c r="C16">
-        <f>B22*(1+$B$7)</f>
-        <v/>
-      </c>
-      <c r="D16">
-        <f>C22*(1+$B$7)</f>
-        <v/>
-      </c>
-      <c r="E16">
-        <f>D22*(1+$B$7)</f>
-        <v/>
-      </c>
-      <c r="F16">
-        <f>E22*(1+$B$7)</f>
-        <v/>
-      </c>
-      <c r="G16">
-        <f>F22*(1+$B$7)</f>
-        <v/>
-      </c>
+        <f>$B$1*$B$15</f>
+        <v/>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EBITDA</t>
+          <t>debt_portion</t>
         </is>
       </c>
       <c r="B17">
-        <f>B22*$B$3</f>
-        <v/>
-      </c>
-      <c r="C17">
-        <f>C22*$B$3</f>
-        <v/>
-      </c>
-      <c r="D17">
-        <f>D22*$B$3</f>
-        <v/>
-      </c>
-      <c r="E17">
-        <f>E22*$B$3</f>
-        <v/>
-      </c>
-      <c r="F17">
-        <f>F22*$B$3</f>
-        <v/>
-      </c>
-      <c r="G17">
-        <f>G22*$B$3</f>
-        <v/>
-      </c>
+        <f>$B$4*$B$16</f>
+        <v/>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>less: D&amp;A</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18">
-        <f>-$B$12</f>
-        <v/>
-      </c>
-      <c r="D18">
-        <f>-$B$12</f>
-        <v/>
-      </c>
-      <c r="E18">
-        <f>-$B$12</f>
-        <v/>
-      </c>
-      <c r="F18">
-        <f>-$B$12</f>
-        <v/>
-      </c>
-      <c r="G18">
-        <f>-$B$12</f>
-        <v/>
-      </c>
+          <t>equity_portion</t>
+        </is>
+      </c>
+      <c r="B18">
+        <f>$B$5*$B$16</f>
+        <v/>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>EBIT</t>
-        </is>
-      </c>
-      <c r="B19">
-        <f>B23+B24</f>
-        <v/>
-      </c>
-      <c r="C19">
-        <f>C23+C24</f>
-        <v/>
-      </c>
-      <c r="D19">
-        <f>D23+D24</f>
-        <v/>
-      </c>
-      <c r="E19">
-        <f>E23+E24</f>
-        <v/>
-      </c>
-      <c r="F19">
-        <f>F23+F24</f>
-        <v/>
-      </c>
-      <c r="G19">
-        <f>G23+G24</f>
-        <v/>
-      </c>
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>less: Interest</t>
-        </is>
-      </c>
-      <c r="B20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
-      <c r="C20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
-      <c r="D20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
-      <c r="E20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
-      <c r="F20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
-      <c r="G20">
-        <f>-$B$8*$B$17</f>
-        <v/>
-      </c>
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EBT</t>
-        </is>
-      </c>
-      <c r="B21">
-        <f>B25+B26</f>
-        <v/>
-      </c>
-      <c r="C21">
-        <f>C25+C26</f>
-        <v/>
-      </c>
-      <c r="D21">
-        <f>D25+D26</f>
-        <v/>
-      </c>
-      <c r="E21">
-        <f>E25+E26</f>
-        <v/>
-      </c>
-      <c r="F21">
-        <f>F25+F26</f>
-        <v/>
-      </c>
-      <c r="G21">
-        <f>G25+G26</f>
-        <v/>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>less: Taxes</t>
+          <t>Rev</t>
         </is>
       </c>
       <c r="B22">
-        <f>B27*-$B$9</f>
+        <f>$B$2</f>
         <v/>
       </c>
       <c r="C22">
-        <f>C27*-$B$9</f>
+        <f>B22*(1+$B$7)</f>
         <v/>
       </c>
       <c r="D22">
-        <f>D27*-$B$9</f>
+        <f>C22*(1+$B$7)</f>
         <v/>
       </c>
       <c r="E22">
-        <f>E27*-$B$9</f>
+        <f>D22*(1+$B$7)</f>
         <v/>
       </c>
       <c r="F22">
-        <f>F27*-$B$9</f>
-        <v/>
-      </c>
-      <c r="G22">
-        <f>G27*-$B$9</f>
+        <f>E22*(1+$B$7)</f>
         <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Earnings</t>
+          <t>EBITDA</t>
         </is>
       </c>
       <c r="B23">
-        <f>B27+B28</f>
+        <f>B22*$B$3</f>
         <v/>
       </c>
       <c r="C23">
-        <f>C27+C28</f>
+        <f>C22*$B$3</f>
         <v/>
       </c>
       <c r="D23">
-        <f>D27+D28</f>
+        <f>D22*$B$3</f>
         <v/>
       </c>
       <c r="E23">
-        <f>E27+E28</f>
+        <f>E22*$B$3</f>
         <v/>
       </c>
       <c r="F23">
-        <f>F27+F28</f>
-        <v/>
-      </c>
-      <c r="G23" t="inlineStr"/>
+        <f>F22*$B$3</f>
+        <v/>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>plus: D&amp;A</t>
+          <t>less: D&amp;A</t>
         </is>
       </c>
       <c r="B24">
-        <f>-B24</f>
+        <f>-$B$12</f>
         <v/>
       </c>
       <c r="C24">
-        <f>-C24</f>
+        <f>-$B$12</f>
         <v/>
       </c>
       <c r="D24">
-        <f>-D24</f>
+        <f>-$B$12</f>
         <v/>
       </c>
       <c r="E24">
-        <f>-E24</f>
+        <f>-$B$12</f>
         <v/>
       </c>
       <c r="F24">
-        <f>-F24</f>
-        <v/>
-      </c>
-      <c r="G24" t="inlineStr"/>
+        <f>-$B$12</f>
+        <v/>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>less: capex</t>
+          <t>EBIT</t>
         </is>
       </c>
       <c r="B25">
-        <f>B22*-$B$10</f>
+        <f>B23+B24</f>
         <v/>
       </c>
       <c r="C25">
-        <f>C22*-$B$10</f>
+        <f>C23+C24</f>
         <v/>
       </c>
       <c r="D25">
-        <f>D22*-$B$10</f>
+        <f>D23+D24</f>
         <v/>
       </c>
       <c r="E25">
-        <f>E22*-$B$10</f>
+        <f>E23+E24</f>
         <v/>
       </c>
       <c r="F25">
-        <f>F22*-$B$10</f>
-        <v/>
-      </c>
-      <c r="G25" t="inlineStr"/>
+        <f>F23+F24</f>
+        <v/>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>less: NWC</t>
+          <t>less: Interest</t>
         </is>
       </c>
       <c r="B26">
-        <f>-$B$11</f>
+        <f>-$B$8*$B$17</f>
         <v/>
       </c>
       <c r="C26">
-        <f>-$B$11</f>
+        <f>-$B$8*$B$17</f>
         <v/>
       </c>
       <c r="D26">
-        <f>-$B$11</f>
+        <f>-$B$8*$B$17</f>
         <v/>
       </c>
       <c r="E26">
-        <f>-$B$11</f>
+        <f>-$B$8*$B$17</f>
         <v/>
       </c>
       <c r="F26">
-        <f>-$B$11</f>
-        <v/>
-      </c>
-      <c r="G26" t="inlineStr"/>
+        <f>-$B$8*$B$17</f>
+        <v/>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FCF</t>
+          <t>EBT</t>
         </is>
       </c>
       <c r="B27">
-        <f>SUM(B29:B32)</f>
+        <f>B25+B26</f>
         <v/>
       </c>
       <c r="C27">
-        <f>SUM(C29:C32)</f>
+        <f>C25+C26</f>
         <v/>
       </c>
       <c r="D27">
-        <f>SUM(D29:D32)</f>
+        <f>D25+D26</f>
         <v/>
       </c>
       <c r="E27">
-        <f>SUM(E29:E32)</f>
+        <f>E25+E26</f>
         <v/>
       </c>
       <c r="F27">
-        <f>SUM(F29:F32)</f>
-        <v/>
-      </c>
-      <c r="G27" t="inlineStr"/>
+        <f>F25+F26</f>
+        <v/>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>less: Taxes</t>
+        </is>
+      </c>
+      <c r="B28">
+        <f>B27*-$B$9</f>
+        <v/>
+      </c>
+      <c r="C28">
+        <f>C27*-$B$9</f>
+        <v/>
+      </c>
+      <c r="D28">
+        <f>D27*-$B$9</f>
+        <v/>
+      </c>
+      <c r="E28">
+        <f>E27*-$B$9</f>
+        <v/>
+      </c>
+      <c r="F28">
+        <f>F27*-$B$9</f>
+        <v/>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Earnings</t>
+        </is>
+      </c>
+      <c r="B29">
+        <f>B27+B28</f>
+        <v/>
+      </c>
+      <c r="C29">
+        <f>C27+C28</f>
+        <v/>
+      </c>
+      <c r="D29">
+        <f>D27+D28</f>
+        <v/>
+      </c>
+      <c r="E29">
+        <f>E27+E28</f>
+        <v/>
+      </c>
       <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>exit_EBITDA</t>
+          <t>plus: D&amp;A</t>
         </is>
       </c>
       <c r="B30">
-        <f>$G$23</f>
-        <v/>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+        <f>-B24</f>
+        <v/>
+      </c>
+      <c r="C30">
+        <f>-C24</f>
+        <v/>
+      </c>
+      <c r="D30">
+        <f>-D24</f>
+        <v/>
+      </c>
+      <c r="E30">
+        <f>-E24</f>
+        <v/>
+      </c>
       <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>exit_multiple</t>
+          <t>less: capex</t>
         </is>
       </c>
       <c r="B31">
-        <f>$B$1</f>
-        <v/>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+        <f>B22*-$B$10</f>
+        <v/>
+      </c>
+      <c r="C31">
+        <f>C22*-$B$10</f>
+        <v/>
+      </c>
+      <c r="D31">
+        <f>D22*-$B$10</f>
+        <v/>
+      </c>
+      <c r="E31">
+        <f>E22*-$B$10</f>
+        <v/>
+      </c>
       <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>beggining_debt</t>
+          <t>less: NWC</t>
         </is>
       </c>
       <c r="B32">
-        <f>$B$17</f>
-        <v/>
-      </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+        <f>-$B$11</f>
+        <v/>
+      </c>
+      <c r="C32">
+        <f>-$B$11</f>
+        <v/>
+      </c>
+      <c r="D32">
+        <f>-$B$11</f>
+        <v/>
+      </c>
+      <c r="E32">
+        <f>-$B$11</f>
+        <v/>
+      </c>
       <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>cumulative_FCF</t>
+          <t>FCF</t>
         </is>
       </c>
       <c r="B33">
-        <f>SUM(B33:F33)</f>
-        <v/>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+        <f>SUM(B29:B32)</f>
+        <v/>
+      </c>
+      <c r="C33">
+        <f>SUM(C29:C32)</f>
+        <v/>
+      </c>
+      <c r="D33">
+        <f>SUM(D29:D32)</f>
+        <v/>
+      </c>
+      <c r="E33">
+        <f>SUM(E29:E32)</f>
+        <v/>
+      </c>
       <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -1151,7 +1053,6 @@
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -1160,71 +1061,142 @@
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>exit_TEV</t>
+          <t>exit_EBITDA</t>
         </is>
       </c>
       <c r="B36">
-        <f>$B$36*$B$37</f>
+        <f>$F$23</f>
         <v/>
       </c>
       <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ending_debt</t>
+          <t>exit_multiple</t>
         </is>
       </c>
       <c r="B37">
-        <f>$B$38-$B$39</f>
+        <f>$B$1</f>
         <v/>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ending_equity</t>
+          <t>beggining_debt</t>
         </is>
       </c>
       <c r="B38">
-        <f>$B$42-$B$43</f>
+        <f>$B$17</f>
         <v/>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MOIC</t>
+          <t>cumulative_FCF</t>
         </is>
       </c>
       <c r="B39">
-        <f>$B$44/$B$18</f>
+        <f>SUM(B33:E33)</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr"/>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr"/>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>exit_TEV</t>
+        </is>
+      </c>
+      <c r="B42">
+        <f>$B$36*$B$37</f>
+        <v/>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ending_debt</t>
+        </is>
+      </c>
+      <c r="B43">
+        <f>$B$38-$B$39</f>
+        <v/>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ending_equity</t>
+        </is>
+      </c>
+      <c r="B44">
+        <f>$B$42-$B$43</f>
+        <v/>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>MOIC</t>
+        </is>
+      </c>
+      <c r="B45">
+        <f>$B$44/$B$18</f>
+        <v/>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>